<commit_message>
First Status Meeting Update
</commit_message>
<xml_diff>
--- a/PoliciesAndDetails/TaskAndEffortSheet.xlsx
+++ b/PoliciesAndDetails/TaskAndEffortSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -102,6 +102,56 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Indian compitors, Global compititors, Growth
+Rate, Revenue Plan.</t>
+  </si>
+  <si>
+    <t>FSD, TSD, Research Doc, Page Design etc. (YTU)</t>
+  </si>
+  <si>
+    <t>Draft version Name and Logo. (My Blogger)</t>
+  </si>
+  <si>
+    <t>For domain name and 
+email no deadlines as of now.</t>
+  </si>
+  <si>
+    <t>page_ID</t>
+  </si>
+  <si>
+    <t>GIT Repository, IDE setup, server, Framework Design
+  Databases, Schema Definition, domain name, email_id, whatsapp group</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Blogger Registration</t>
+  </si>
+  <si>
+    <t>Blogger Home Page</t>
+  </si>
+  <si>
+    <t>Order Page</t>
+  </si>
+  <si>
+    <t>Few Pages design completed(home, blogger, )</t>
+  </si>
+  <si>
+    <t>Validations</t>
+  </si>
+  <si>
+    <t>YTD</t>
+  </si>
+  <si>
+    <t>Meeting Plan</t>
+  </si>
+  <si>
+    <t>1. Daily Status Plan
+2. Product Design(every Sunday and Wednesday)
+3. Revenue Plan</t>
   </si>
 </sst>
 </file>
@@ -178,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -188,6 +238,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,12 +538,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -497,13 +587,13 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -572,8 +662,12 @@
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="3">
+        <v>42294</v>
+      </c>
+      <c r="E3" s="7">
+        <v>42299</v>
+      </c>
       <c r="F3" s="6" t="s">
         <v>27</v>
       </c>
@@ -588,8 +682,12 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="3">
+        <v>42299</v>
+      </c>
+      <c r="E4" s="3">
+        <v>42308</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>27</v>
       </c>
@@ -600,11 +698,15 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="3">
+        <v>42291</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="6" t="s">
         <v>27</v>
@@ -616,12 +718,18 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="3">
+        <v>42294</v>
+      </c>
+      <c r="E6" s="3">
+        <v>42307</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>27</v>
       </c>
@@ -650,7 +758,9 @@
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
@@ -662,47 +772,79 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="60">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="6" t="s">
-        <v>27</v>
+      <c r="D9" s="3">
+        <v>42294</v>
+      </c>
+      <c r="E9" s="3">
+        <v>42299</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.2</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3">
+        <v>42294</v>
+      </c>
+      <c r="E10" s="3">
+        <v>42299</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>42294</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+    <row r="12" spans="1:8" ht="45">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>

</xml_diff>